<commit_message>
algorithm-28 셔틀버스 - 수정
</commit_message>
<xml_diff>
--- a/src/main/java/kr/co/programmers/P17678.xlsx
+++ b/src/main/java/kr/co/programmers/P17678.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\projects\algorithm\src\main\java\kr\co\programmers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C39499-6E72-4350-9B4D-72197E4EF772}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F2B1214-D834-40EB-A522-F1B5C6206FCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5070" yWindow="705" windowWidth="17505" windowHeight="12885" xr2:uid="{C83BA903-54C4-4AAD-9479-242F568125DF}"/>
   </bookViews>
@@ -259,12 +259,6 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -272,6 +266,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -590,8 +590,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F7A8E64-2D52-461D-A579-4C246A620175}">
   <dimension ref="B3:K45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="M41" sqref="M41"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="I19" sqref="I18:I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.625" defaultRowHeight="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -638,10 +638,10 @@
       <c r="G4" s="4"/>
     </row>
     <row r="5" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="6"/>
+      <c r="E5" s="8"/>
     </row>
     <row r="6" spans="2:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="3" t="s">
@@ -679,7 +679,7 @@
       <c r="F7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="7" t="s">
+      <c r="G7" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -727,7 +727,7 @@
         <v>11</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>11</v>
@@ -736,12 +736,12 @@
         <v>11</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H14" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="H14" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I14" s="6" t="s">
         <v>11</v>
       </c>
     </row>
@@ -781,7 +781,7 @@
       <c r="F19" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G19" s="7" t="s">
+      <c r="G19" s="5" t="s">
         <v>16</v>
       </c>
       <c r="H19" s="2" t="s">
@@ -807,7 +807,7 @@
       <c r="H20" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I20" s="9" t="s">
+      <c r="I20" s="7" t="s">
         <v>6</v>
       </c>
     </row>
@@ -852,10 +852,10 @@
       </c>
     </row>
     <row r="26" spans="2:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E26" s="6"/>
+      <c r="E26" s="8"/>
     </row>
     <row r="27" spans="2:9" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="3" t="s">
@@ -881,7 +881,7 @@
       <c r="B28" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C28" s="7" t="s">
+      <c r="C28" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D28" s="2" t="s">
@@ -904,7 +904,7 @@
       <c r="C32" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E32" s="5" t="s">
+      <c r="E32" s="9" t="s">
         <v>14</v>
       </c>
       <c r="F32" s="3" t="s">
@@ -919,17 +919,17 @@
         <v>6</v>
       </c>
       <c r="C33" s="2"/>
-      <c r="D33" s="9" t="s">
+      <c r="D33" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="E33" s="5"/>
+      <c r="E33" s="9"/>
       <c r="F33" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G33" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="H33" s="9" t="s">
+      <c r="G33" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="H33" s="7" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1004,7 +1004,7 @@
         <v>11</v>
       </c>
       <c r="I39" s="2"/>
-      <c r="J39" s="7" t="s">
+      <c r="J39" s="5" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1061,7 +1061,7 @@
       <c r="D45" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E45" s="8" t="s">
+      <c r="E45" s="6" t="s">
         <v>11</v>
       </c>
       <c r="G45" s="3" t="s">
@@ -1070,13 +1070,13 @@
       <c r="H45" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I45" s="7" t="s">
+      <c r="I45" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="J45" s="9" t="s">
+      <c r="J45" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="K45" s="9" t="s">
+      <c r="K45" s="7" t="s">
         <v>11</v>
       </c>
     </row>

</xml_diff>